<commit_message>
update context table and add code
</commit_message>
<xml_diff>
--- a/Context table for openaps.xlsx
+++ b/Context table for openaps.xlsx
@@ -171,16 +171,13 @@
   <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.2959183673469"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.6224489795918"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
edit fault injection code and context table.
</commit_message>
<xml_diff>
--- a/Context table for openaps.xlsx
+++ b/Context table for openaps.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t xml:space="preserve">glucose &lt; bg_target</t>
   </si>
@@ -58,10 +58,16 @@
     <t xml:space="preserve">loaded_suggested_data["rate"] = [0,0.2]</t>
   </si>
   <si>
+    <t xml:space="preserve">loaded_glucose &lt; 120</t>
+  </si>
+  <si>
     <t xml:space="preserve">data_to_prepend["glucose"] += x</t>
   </si>
   <si>
     <t xml:space="preserve">data_to_prepend["glucose"] = [120,350]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loaded_glucose &gt; 120</t>
   </si>
   <si>
     <t xml:space="preserve">data_to_prepend["glucose"] -= x</t>
@@ -171,13 +177,16 @@
   <dimension ref="A2:F9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.6224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="49.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -241,10 +250,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>3</v>
@@ -258,7 +267,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -266,13 +275,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>9</v>
@@ -286,7 +295,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>